<commit_message>
test data modified , added user_mobile for revoke license
</commit_message>
<xml_diff>
--- a/TestData/Production/AdminConsole/Promo/promo_test_data.xlsx
+++ b/TestData/Production/AdminConsole/Promo/promo_test_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saloni\Desktop\Ginesys\Ginesys Zwing\Ginesys_Zwing_Automation\TestData\AdminConsole\Promo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saloni\Desktop\Ginesys\Zwing_repo\zwing-qa-automation\TestData\Production\AdminConsole\Promo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -105,7 +105,7 @@
     <t>TC-01</t>
   </si>
   <si>
-    <t>zwshashank.agrawal@teampureplay.com</t>
+    <t>Zwingautomation78@gmail.com</t>
   </si>
   <si>
     <t>QBSB-any___qty-Flat-Percentage</t>
@@ -1085,8 +1085,8 @@
     <outlinePr summaryRight="0" summaryBelow="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A61">
-      <selection activeCell="D78" sqref="D78"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
@@ -1215,7 +1215,7 @@
         <v>28</v>
       </c>
       <c r="C3" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>29</v>
@@ -1286,7 +1286,7 @@
         <v>28</v>
       </c>
       <c r="C4" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>39</v>
@@ -1357,7 +1357,7 @@
         <v>28</v>
       </c>
       <c r="C5" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>42</v>
@@ -1428,7 +1428,7 @@
         <v>28</v>
       </c>
       <c r="C6" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>46</v>
@@ -1499,7 +1499,7 @@
         <v>28</v>
       </c>
       <c r="C7" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>51</v>
@@ -1570,7 +1570,7 @@
         <v>28</v>
       </c>
       <c r="C8" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>57</v>
@@ -1641,7 +1641,7 @@
         <v>28</v>
       </c>
       <c r="C9" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>63</v>
@@ -1712,7 +1712,7 @@
         <v>28</v>
       </c>
       <c r="C10" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>66</v>
@@ -1783,7 +1783,7 @@
         <v>28</v>
       </c>
       <c r="C11" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>71</v>
@@ -1854,7 +1854,7 @@
         <v>28</v>
       </c>
       <c r="C12" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>74</v>
@@ -1925,7 +1925,7 @@
         <v>28</v>
       </c>
       <c r="C13" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>78</v>
@@ -1996,7 +1996,7 @@
         <v>28</v>
       </c>
       <c r="C14" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>81</v>
@@ -2067,7 +2067,7 @@
         <v>28</v>
       </c>
       <c r="C15" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>84</v>
@@ -2138,7 +2138,7 @@
         <v>28</v>
       </c>
       <c r="C16" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>87</v>
@@ -2209,7 +2209,7 @@
         <v>28</v>
       </c>
       <c r="C17" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>90</v>
@@ -2280,7 +2280,7 @@
         <v>28</v>
       </c>
       <c r="C18" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>93</v>
@@ -2351,7 +2351,7 @@
         <v>28</v>
       </c>
       <c r="C19" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>96</v>
@@ -2422,7 +2422,7 @@
         <v>28</v>
       </c>
       <c r="C20" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>99</v>
@@ -2493,7 +2493,7 @@
         <v>28</v>
       </c>
       <c r="C21" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>103</v>
@@ -2564,7 +2564,7 @@
         <v>28</v>
       </c>
       <c r="C22" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>106</v>
@@ -2635,7 +2635,7 @@
         <v>28</v>
       </c>
       <c r="C23" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>109</v>
@@ -2706,7 +2706,7 @@
         <v>28</v>
       </c>
       <c r="C24" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>112</v>
@@ -2777,7 +2777,7 @@
         <v>28</v>
       </c>
       <c r="C25" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>115</v>
@@ -2848,7 +2848,7 @@
         <v>28</v>
       </c>
       <c r="C26" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>118</v>
@@ -2919,7 +2919,7 @@
         <v>28</v>
       </c>
       <c r="C27" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>121</v>
@@ -2990,7 +2990,7 @@
         <v>28</v>
       </c>
       <c r="C28" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>124</v>
@@ -3061,7 +3061,7 @@
         <v>28</v>
       </c>
       <c r="C29" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>127</v>
@@ -3132,7 +3132,7 @@
         <v>28</v>
       </c>
       <c r="C30" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>130</v>
@@ -3203,7 +3203,7 @@
         <v>28</v>
       </c>
       <c r="C31" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>135</v>
@@ -3274,7 +3274,7 @@
         <v>28</v>
       </c>
       <c r="C32" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>138</v>
@@ -3345,7 +3345,7 @@
         <v>28</v>
       </c>
       <c r="C33" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>141</v>
@@ -3416,7 +3416,7 @@
         <v>28</v>
       </c>
       <c r="C34" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>144</v>
@@ -3487,7 +3487,7 @@
         <v>28</v>
       </c>
       <c r="C35" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>147</v>
@@ -3558,7 +3558,7 @@
         <v>28</v>
       </c>
       <c r="C36" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>150</v>
@@ -3629,7 +3629,7 @@
         <v>28</v>
       </c>
       <c r="C37" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>153</v>
@@ -3700,7 +3700,7 @@
         <v>28</v>
       </c>
       <c r="C38" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>156</v>
@@ -3771,7 +3771,7 @@
         <v>28</v>
       </c>
       <c r="C39" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>159</v>
@@ -3842,7 +3842,7 @@
         <v>28</v>
       </c>
       <c r="C40" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>162</v>
@@ -3913,7 +3913,7 @@
         <v>28</v>
       </c>
       <c r="C41" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>165</v>
@@ -3984,7 +3984,7 @@
         <v>28</v>
       </c>
       <c r="C42" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>168</v>
@@ -4055,7 +4055,7 @@
         <v>28</v>
       </c>
       <c r="C43" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>171</v>
@@ -4126,7 +4126,7 @@
         <v>28</v>
       </c>
       <c r="C44" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>174</v>
@@ -4197,7 +4197,7 @@
         <v>28</v>
       </c>
       <c r="C45" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>177</v>
@@ -4268,7 +4268,7 @@
         <v>28</v>
       </c>
       <c r="C46" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>180</v>
@@ -4339,7 +4339,7 @@
         <v>28</v>
       </c>
       <c r="C47" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>183</v>
@@ -4410,7 +4410,7 @@
         <v>28</v>
       </c>
       <c r="C48" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>186</v>
@@ -4481,7 +4481,7 @@
         <v>28</v>
       </c>
       <c r="C49" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>189</v>
@@ -4552,7 +4552,7 @@
         <v>28</v>
       </c>
       <c r="C50" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>192</v>
@@ -4623,7 +4623,7 @@
         <v>28</v>
       </c>
       <c r="C51" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>198</v>
@@ -4694,7 +4694,7 @@
         <v>28</v>
       </c>
       <c r="C52" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>202</v>
@@ -4765,7 +4765,7 @@
         <v>28</v>
       </c>
       <c r="C53" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>206</v>
@@ -4836,7 +4836,7 @@
         <v>28</v>
       </c>
       <c r="C54" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>209</v>
@@ -4907,7 +4907,7 @@
         <v>28</v>
       </c>
       <c r="C55" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>212</v>
@@ -4978,7 +4978,7 @@
         <v>28</v>
       </c>
       <c r="C56" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>215</v>
@@ -5049,7 +5049,7 @@
         <v>28</v>
       </c>
       <c r="C57" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>218</v>
@@ -5120,7 +5120,7 @@
         <v>28</v>
       </c>
       <c r="C58" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>221</v>
@@ -5191,7 +5191,7 @@
         <v>28</v>
       </c>
       <c r="C59" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>224</v>
@@ -5262,7 +5262,7 @@
         <v>28</v>
       </c>
       <c r="C60" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>227</v>
@@ -5333,7 +5333,7 @@
         <v>28</v>
       </c>
       <c r="C61" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>230</v>
@@ -5404,7 +5404,7 @@
         <v>28</v>
       </c>
       <c r="C62" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>233</v>
@@ -5475,7 +5475,7 @@
         <v>28</v>
       </c>
       <c r="C63" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>236</v>
@@ -5546,7 +5546,7 @@
         <v>28</v>
       </c>
       <c r="C64" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>240</v>
@@ -5617,7 +5617,7 @@
         <v>28</v>
       </c>
       <c r="C65" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>244</v>
@@ -5685,7 +5685,7 @@
         <v>28</v>
       </c>
       <c r="C66" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>247</v>
@@ -5753,7 +5753,7 @@
         <v>28</v>
       </c>
       <c r="C67" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>249</v>
@@ -5821,7 +5821,7 @@
         <v>28</v>
       </c>
       <c r="C68" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>251</v>
@@ -5889,7 +5889,7 @@
         <v>28</v>
       </c>
       <c r="C69" s="2">
-        <v>123456</v>
+        <v>1234</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>254</v>

</xml_diff>